<commit_message>
seo probuilds blogs optimized
</commit_message>
<xml_diff>
--- a/private/concepts/seo/static/lolvvv/lolvvv - Web20 - {championName} Probuilds - 5847323.xlsx
+++ b/private/concepts/seo/static/lolvvv/lolvvv - Web20 - {championName} Probuilds - 5847323.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D16FD1E-B3C2-40A9-83E2-8BC709B8871D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E584385-84C6-4789-8D76-54D4D4096EB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="3855" windowWidth="25065" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1965" yWindow="1605" windowWidth="16605" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="79">
   <si>
     <t>WEB 2.0 BLOG</t>
   </si>
@@ -385,7 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -464,14 +464,21 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -815,46 +822,53 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="62.42578125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="36" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="47.7109375" style="25" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="25"/>
+    <col min="10" max="10" width="9.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:10" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -868,19 +882,19 @@
       <c r="E4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I4" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="34" t="s">
         <v>78</v>
       </c>
     </row>
@@ -900,7 +914,10 @@
       <c r="E5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="1" t="b">
+      <c r="G5" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="32" t="b">
         <v>1</v>
       </c>
     </row>
@@ -920,7 +937,10 @@
       <c r="E6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="1" t="b">
+      <c r="G6" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="32" t="b">
         <v>1</v>
       </c>
     </row>
@@ -940,6 +960,9 @@
       <c r="E7" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="H7" s="32" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
@@ -957,7 +980,10 @@
       <c r="E8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="1" t="b">
+      <c r="G8" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="32" t="b">
         <v>1</v>
       </c>
     </row>
@@ -977,7 +1003,10 @@
       <c r="E9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="1" t="b">
+      <c r="G9" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="32" t="b">
         <v>1</v>
       </c>
     </row>
@@ -997,7 +1026,10 @@
       <c r="E10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="1" t="b">
+      <c r="G10" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="32" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1017,6 +1049,9 @@
       <c r="E11" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="H11" s="25" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
@@ -1034,6 +1069,15 @@
       <c r="E12" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="G12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="25" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
@@ -1051,6 +1095,18 @@
       <c r="E13" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="F13" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="25" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
@@ -1068,7 +1124,10 @@
       <c r="E14" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J14" s="1" t="b">
+      <c r="H14" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="25" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1088,6 +1147,9 @@
       <c r="E15" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="H15" s="25" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
@@ -1105,8 +1167,11 @@
       <c r="E16" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H16" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>26</v>
       </c>
@@ -1122,8 +1187,11 @@
       <c r="E17" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H17" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>15</v>
       </c>
@@ -1139,8 +1207,11 @@
       <c r="E18" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H18" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>22</v>
       </c>
@@ -1156,8 +1227,17 @@
       <c r="E19" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G19" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -1173,8 +1253,17 @@
       <c r="E20" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G20" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
@@ -1190,8 +1279,11 @@
       <c r="E21" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1207,8 +1299,17 @@
       <c r="E22" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G22" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>20</v>
       </c>
@@ -1224,11 +1325,17 @@
       <c r="E23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G23" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G23" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>21</v>
       </c>
@@ -1244,18 +1351,27 @@
       <c r="E24" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G24" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C25" s="29"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C26" s="29"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C27" s="29"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>1</v>
       </c>
@@ -1267,20 +1383,23 @@
       <c r="E28" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F28" s="30" t="s">
+      <c r="F28" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="G28" s="30" t="s">
+      <c r="G28" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="H28" s="30" t="s">
+      <c r="H28" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="I28" s="30" t="s">
+      <c r="I28" s="34" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28" s="34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>17</v>
       </c>
@@ -1296,8 +1415,17 @@
       <c r="E29" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G29" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="26" t="s">
         <v>12</v>
       </c>
@@ -1313,8 +1441,17 @@
       <c r="E30" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G30" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -1330,8 +1467,11 @@
       <c r="E31" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H31" s="32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>23</v>
       </c>
@@ -1347,8 +1487,17 @@
       <c r="E32" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G32" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>9</v>
       </c>
@@ -1364,8 +1513,17 @@
       <c r="E33" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G33" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>24</v>
       </c>
@@ -1381,8 +1539,17 @@
       <c r="E34" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G34" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
         <v>7</v>
       </c>
@@ -1398,8 +1565,11 @@
       <c r="E35" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H35" s="32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>4</v>
       </c>
@@ -1415,8 +1585,17 @@
       <c r="E36" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G36" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>13</v>
       </c>
@@ -1432,8 +1611,14 @@
       <c r="E37" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="G37" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" s="32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>10</v>
       </c>
@@ -1449,8 +1634,11 @@
       <c r="E38" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J38" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>8</v>
       </c>
@@ -1466,8 +1654,11 @@
       <c r="E39" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H39" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>11</v>
       </c>
@@ -1483,8 +1674,17 @@
       <c r="E40" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G40" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>26</v>
       </c>
@@ -1500,8 +1700,11 @@
       <c r="E41" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="H41" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>15</v>
       </c>
@@ -1517,8 +1720,11 @@
       <c r="E42" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H42" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>22</v>
       </c>
@@ -1534,8 +1740,17 @@
       <c r="E43" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G43" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>18</v>
       </c>
@@ -1551,8 +1766,11 @@
       <c r="E44" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="H44" s="32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>19</v>
       </c>
@@ -1568,8 +1786,11 @@
       <c r="E45" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J45" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>14</v>
       </c>
@@ -1585,8 +1806,14 @@
       <c r="E46" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" s="25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>20</v>
       </c>
@@ -1596,14 +1823,26 @@
       <c r="C47" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="35" t="s">
         <v>51</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G47" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" s="25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
         <v>21</v>
       </c>
@@ -1618,6 +1857,15 @@
       </c>
       <c r="E48" s="7" t="s">
         <v>5</v>
+      </c>
+      <c r="G48" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I48" s="25" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1626,8 +1874,11 @@
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D47" r:id="rId1" xr:uid="{E1428CA7-30F3-4820-B19C-941F81B2F2CE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
seo blogs excel extended
</commit_message>
<xml_diff>
--- a/private/concepts/seo/static/lolvvv/lolvvv - Web20 - {championName} Probuilds - 5847323.xlsx
+++ b/private/concepts/seo/static/lolvvv/lolvvv - Web20 - {championName} Probuilds - 5847323.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E584385-84C6-4789-8D76-54D4D4096EB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493AAFD8-3E57-40F4-8DCE-1648B38760FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1965" yWindow="1605" windowWidth="16605" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21720" yWindow="795" windowWidth="27825" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="99">
   <si>
     <t>WEB 2.0 BLOG</t>
   </si>
@@ -257,6 +257,66 @@
   </si>
   <si>
     <t>Suspended</t>
+  </si>
+  <si>
+    <t>Blog Article #1</t>
+  </si>
+  <si>
+    <t>Blog Article #2</t>
+  </si>
+  <si>
+    <t>https://kaisa-probuilds.wixsite.com/kaisa-probuilds/post/probuilds-2021-the-most-popular-champions-of-this-lec</t>
+  </si>
+  <si>
+    <t>https://gnarprobuilds.wordpress.com/2021/02/05/five-of-the-best-champion-probuilds-picks-plays-and-stats/</t>
+  </si>
+  <si>
+    <t>https://camille-probuilds.my-free.website/blog/post/239622/2020-probuilds-the-most-dominant-supports</t>
+  </si>
+  <si>
+    <t>https://kidblog.org/class/taliyah-probuilds/posts/efj2seeosdzb2ca8l1kh87acf</t>
+  </si>
+  <si>
+    <t>https://alistar-probuilds.mystrikingly.com</t>
+  </si>
+  <si>
+    <t>https://apheliosprobuilds.shutterfly.com</t>
+  </si>
+  <si>
+    <t>https://rell-probuilds.doodlekit.com/blog/entry/13141979/end-of-an-era-alook-back-in-jinx-probuilds-incredible-career-in-europe-</t>
+  </si>
+  <si>
+    <t>https://samira-probuilds.sitey.me/blog/post/239922/on-the-brink-of-losing-a-moment-with-samira-probuilds</t>
+  </si>
+  <si>
+    <t>https://6013ef656dd92.site123.me/blog/2020-in-review-the-most-dominant-midlaners-of-this-rell-probuilds</t>
+  </si>
+  <si>
+    <t>http://seraphine-probuilds.jigsy.com/entries/general/seraphine-probuilds-a-look-back-in-perkz</t>
+  </si>
+  <si>
+    <t>https://gnarprobuilds.wixsite.com/gnar-probuilds/post/gnar-probuilds-2020-proves-that-g2-s-best-is-yet-to-come</t>
+  </si>
+  <si>
+    <t>https://kaisaprobuilds.wordpress.com/2021/01/29/2020-in-review-the-most-popular-champions-of-this-lec/</t>
+  </si>
+  <si>
+    <t>https://camille-probuilds1.my-free.website/blog/post/240151/camille-probuilds-the-most-dominant-junglers</t>
+  </si>
+  <si>
+    <t>https://kidblog.org/class/samira-probuilds/posts/62eepenx4zknj581inouc5n60</t>
+  </si>
+  <si>
+    <t>https://apheliosprobuilds.doodlekit.com/blog/entry/13165554/end-of-an-era-a-look-back-in-aphelios-probuilds-incredible-career-at-europe-</t>
+  </si>
+  <si>
+    <t>https://kaisaprobuilds.jimdofree.com/2021/01/30/2020-in-review-the-most-dominat-junglers-of-this-lec/</t>
+  </si>
+  <si>
+    <t>https://samira-probuilds21.sitey.me/blog/post/241947/losing-a-moment-for-lol-samira-probuilds</t>
+  </si>
+  <si>
+    <t>http://nidalee-probuilds.jigsy.com/entries/general/nidalee-probuilds-the-one-lol-champion</t>
   </si>
 </sst>
 </file>
@@ -315,14 +375,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1" tint="4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -347,6 +399,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -383,9 +443,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -415,20 +475,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -438,48 +492,55 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -820,25 +881,26 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="47.7109375" style="25" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" style="22" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="25"/>
-    <col min="10" max="10" width="9.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="9" width="9.140625" style="22"/>
+    <col min="10" max="10" width="9.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="22.42578125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>28</v>
       </c>
@@ -847,7 +909,7 @@
       <c r="D1" s="31"/>
       <c r="E1" s="31"/>
     </row>
-    <row r="2" spans="1:10" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>16</v>
       </c>
@@ -856,7 +918,7 @@
       <c r="D2" s="31"/>
       <c r="E2" s="31"/>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>0</v>
       </c>
@@ -864,22 +926,22 @@
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-    </row>
-    <row r="4" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="11" t="s">
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+    </row>
+    <row r="4" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="34" t="s">
@@ -897,15 +959,21 @@
       <c r="J4" s="34" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="L4" s="34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="8">
         <v>99</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="10" t="s">
@@ -914,21 +982,24 @@
       <c r="E5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="G5" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="18">
         <v>94</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="24" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -937,21 +1008,24 @@
       <c r="E6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G6" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="5">
         <v>95</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="24" t="s">
         <v>31</v>
       </c>
       <c r="D7" s="10" t="s">
@@ -960,18 +1034,18 @@
       <c r="E7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="H7" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="5">
         <v>82</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="24" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="10" t="s">
@@ -980,21 +1054,24 @@
       <c r="E8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" s="32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G8" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="18">
         <v>92</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="24" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="10" t="s">
@@ -1003,21 +1080,24 @@
       <c r="E9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" s="32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
+      <c r="G9" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="14">
         <v>82</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="10" t="s">
@@ -1026,21 +1106,27 @@
       <c r="E10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" s="32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="G10" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="18">
         <v>79</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="24" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="10" t="s">
@@ -1049,18 +1135,18 @@
       <c r="E11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="25" t="b">
+      <c r="H11" s="22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="9">
         <v>69</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="24" t="s">
         <v>36</v>
       </c>
       <c r="D12" s="10" t="s">
@@ -1069,24 +1155,27 @@
       <c r="E12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="25" t="b">
+      <c r="G12" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
+      <c r="K12" s="36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="14">
         <v>95</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="24" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="10" t="s">
@@ -1095,27 +1184,30 @@
       <c r="E13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F13" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" s="18">
         <v>79</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="24" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="10" t="s">
@@ -1124,21 +1216,21 @@
       <c r="E14" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="25" t="b">
+      <c r="H14" s="22" t="b">
         <v>0</v>
       </c>
-      <c r="J14" s="25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J14" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="9">
         <v>73</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="10" t="s">
@@ -1147,18 +1239,18 @@
       <c r="E15" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="25" t="b">
+      <c r="H15" s="22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="5">
         <v>91</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="24" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="10" t="s">
@@ -1167,18 +1259,18 @@
       <c r="E16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="25" t="b">
+      <c r="H16" s="22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="19">
         <v>68</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="24" t="s">
         <v>42</v>
       </c>
       <c r="D17" s="10" t="s">
@@ -1187,18 +1279,18 @@
       <c r="E17" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="25" t="b">
+      <c r="H17" s="22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="10">
         <v>75</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D18" s="10" t="s">
@@ -1207,18 +1299,18 @@
       <c r="E18" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H18" s="25" t="b">
+      <c r="H18" s="22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="20">
         <v>57</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="24" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="10" t="s">
@@ -1227,24 +1319,27 @@
       <c r="E19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" s="32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G19" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="11">
         <v>67</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="25" t="s">
         <v>45</v>
       </c>
       <c r="D20" s="10" t="s">
@@ -1253,24 +1348,27 @@
       <c r="E20" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" s="25" t="b">
+      <c r="G20" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="11">
         <v>87</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="24" t="s">
         <v>47</v>
       </c>
       <c r="D21" s="10" t="s">
@@ -1279,18 +1377,18 @@
       <c r="E21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J21" s="25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J21" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="3">
         <v>54</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="24" t="s">
         <v>48</v>
       </c>
       <c r="D22" s="10" t="s">
@@ -1299,24 +1397,27 @@
       <c r="E22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H22" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I22" s="32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G22" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="3">
         <v>47</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="24" t="s">
         <v>49</v>
       </c>
       <c r="D23" s="10" t="s">
@@ -1325,24 +1426,27 @@
       <c r="E23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G23" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H23" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I23" s="32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="14" t="s">
+      <c r="G23" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="22">
+      <c r="B24" s="20">
         <v>42</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="25" t="s">
         <v>50</v>
       </c>
       <c r="D24" s="10" t="s">
@@ -1351,36 +1455,39 @@
       <c r="E24" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H24" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I24" s="25" t="b">
+      <c r="G24" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C25" s="29"/>
+      <c r="K24" s="25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C25" s="26"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C26" s="29"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C27" s="29"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="11" t="s">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C26" s="26"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C27" s="26"/>
+    </row>
+    <row r="28" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11" t="s">
+      <c r="C28" s="33"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32" t="s">
         <v>3</v>
       </c>
       <c r="F28" s="34" t="s">
@@ -1398,8 +1505,14 @@
       <c r="J28" s="34" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="L28" s="34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>17</v>
       </c>
@@ -1415,24 +1528,27 @@
       <c r="E29" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G29" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H29" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I29" s="25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="26" t="s">
+      <c r="G29" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="20">
+      <c r="B30" s="18">
         <v>94</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="24" t="s">
         <v>53</v>
       </c>
       <c r="D30" s="10" t="s">
@@ -1441,24 +1557,27 @@
       <c r="E30" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H30" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I30" s="25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G30" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B31" s="5">
         <v>95</v>
       </c>
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="24" t="s">
         <v>54</v>
       </c>
       <c r="D31" s="10" t="s">
@@ -1467,18 +1586,18 @@
       <c r="E31" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H31" s="32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="14" t="s">
+      <c r="H31" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B32" s="5">
         <v>82</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="24" t="s">
         <v>55</v>
       </c>
       <c r="D32" s="10" t="s">
@@ -1487,24 +1606,27 @@
       <c r="E32" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G32" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H32" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I32" s="25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G32" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="20">
+      <c r="B33" s="18">
         <v>92</v>
       </c>
-      <c r="C33" s="27" t="s">
+      <c r="C33" s="24" t="s">
         <v>56</v>
       </c>
       <c r="D33" s="10" t="s">
@@ -1513,24 +1635,27 @@
       <c r="E33" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H33" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I33" s="25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="14" t="s">
+      <c r="G33" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="16">
+      <c r="B34" s="14">
         <v>82</v>
       </c>
-      <c r="C34" s="27" t="s">
+      <c r="C34" s="24" t="s">
         <v>57</v>
       </c>
       <c r="D34" s="10" t="s">
@@ -1539,24 +1664,27 @@
       <c r="E34" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G34" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H34" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I34" s="25" t="b">
+      <c r="G34" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" s="22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="15" t="s">
+      <c r="K34" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="20">
+      <c r="B35" s="18">
         <v>79</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="C35" s="24" t="s">
         <v>58</v>
       </c>
       <c r="D35" s="10" t="s">
@@ -1565,18 +1693,18 @@
       <c r="E35" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H35" s="32" t="b">
+      <c r="H35" s="27" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="14" t="s">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B36" s="9">
         <v>69</v>
       </c>
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="24" t="s">
         <v>59</v>
       </c>
       <c r="D36" s="10" t="s">
@@ -1585,24 +1713,27 @@
       <c r="E36" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G36" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I36" s="25" t="b">
+      <c r="G36" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" s="22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="17" t="s">
+      <c r="K36" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="16">
+      <c r="B37" s="14">
         <v>95</v>
       </c>
-      <c r="C37" s="27" t="s">
+      <c r="C37" s="24" t="s">
         <v>60</v>
       </c>
       <c r="D37" s="10" t="s">
@@ -1611,41 +1742,47 @@
       <c r="E37" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G37" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" s="32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="G37" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K37" s="24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="20">
+      <c r="B38" s="18">
         <v>79</v>
       </c>
-      <c r="C38" s="27" t="s">
+      <c r="C38" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="21" t="s">
         <v>61</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J38" s="25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J38" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B39" s="9">
         <v>73</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="C39" s="24" t="s">
         <v>63</v>
       </c>
       <c r="D39" s="10" t="s">
@@ -1654,18 +1791,18 @@
       <c r="E39" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H39" s="25" t="b">
+      <c r="H39" s="22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B40" s="5">
         <v>91</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="24" t="s">
         <v>64</v>
       </c>
       <c r="D40" s="10" t="s">
@@ -1674,24 +1811,27 @@
       <c r="E40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G40" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H40" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I40" s="25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G40" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K40" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="21">
+      <c r="B41" s="19">
         <v>68</v>
       </c>
-      <c r="C41" s="27" t="s">
+      <c r="C41" s="24" t="s">
         <v>65</v>
       </c>
       <c r="D41" s="10" t="s">
@@ -1700,38 +1840,38 @@
       <c r="E41" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H41" s="25" t="b">
+      <c r="H41" s="22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B42" s="10">
         <v>75</v>
       </c>
-      <c r="C42" s="27" t="s">
+      <c r="C42" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="D42" s="23" t="s">
+      <c r="D42" s="21" t="s">
         <v>61</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H42" s="25" t="b">
+      <c r="H42" s="22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="22">
+      <c r="B43" s="20">
         <v>57</v>
       </c>
-      <c r="C43" s="27" t="s">
+      <c r="C43" s="24" t="s">
         <v>67</v>
       </c>
       <c r="D43" s="10" t="s">
@@ -1740,24 +1880,27 @@
       <c r="E43" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G43" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H43" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I43" s="25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G43" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="13">
+      <c r="B44" s="11">
         <v>67</v>
       </c>
-      <c r="C44" s="29" t="s">
+      <c r="C44" s="26" t="s">
         <v>68</v>
       </c>
       <c r="D44" s="10" t="s">
@@ -1766,38 +1909,38 @@
       <c r="E44" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H44" s="32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="H44" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="13">
+      <c r="B45" s="11">
         <v>87</v>
       </c>
-      <c r="C45" s="27" t="s">
+      <c r="C45" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D45" s="23" t="s">
+      <c r="D45" s="21" t="s">
         <v>69</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J45" s="25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J45" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B46" s="3">
         <v>54</v>
       </c>
-      <c r="C46" s="27" t="s">
+      <c r="C46" s="24" t="s">
         <v>71</v>
       </c>
       <c r="D46" s="10" t="s">
@@ -1806,50 +1949,53 @@
       <c r="E46" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H46" s="25" t="b">
+      <c r="F46" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" s="22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B47" s="3">
         <v>47</v>
       </c>
-      <c r="C47" s="27" t="s">
+      <c r="C47" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D47" s="35" t="s">
+      <c r="D47" s="29" t="s">
         <v>51</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="G47" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H47" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I47" s="25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="14" t="s">
+      <c r="F47" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G47" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B48" s="22">
+      <c r="B48" s="20">
         <v>42</v>
       </c>
-      <c r="C48" s="29" t="s">
+      <c r="C48" s="26" t="s">
         <v>73</v>
       </c>
       <c r="D48" s="10" t="s">
@@ -1858,14 +2004,17 @@
       <c r="E48" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G48" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H48" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I48" s="25" t="b">
+      <c r="G48" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I48" s="22" t="b">
         <v>0</v>
+      </c>
+      <c r="K48" s="26" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>